<commit_message>
added the different methods to the trade simulator
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/HZNP/HZNPBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/HZNP/HZNPBag.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualStudioProjects\StockPredictor\StockPredictor\bin\Debug\packages\Data\HZNP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualStudioProjects\StockPredictor\StockPredictor\bin\Debug\Packages\Data\HZNP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -384,9 +384,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:H5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -489,247 +491,124 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>42600.792164351849</v>
+        <v>42600.879189814812</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3">
-        <v>6409</v>
+        <v>5830</v>
       </c>
       <c r="D3">
-        <v>9671</v>
+        <v>6498</v>
       </c>
       <c r="E3">
-        <v>1129</v>
+        <v>754</v>
       </c>
       <c r="F3">
-        <v>161</v>
+        <v>73</v>
       </c>
       <c r="G3">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H3">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="I3">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
       <c r="L3">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="M3">
-        <v>33</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>42600.794490740744</v>
+        <v>42602.582511574074</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4">
-        <v>8579</v>
+        <v>6203</v>
       </c>
       <c r="D4">
-        <v>11114</v>
+        <v>9316</v>
       </c>
       <c r="E4">
-        <v>1326</v>
+        <v>1145</v>
       </c>
       <c r="F4">
-        <v>175</v>
+        <v>133</v>
       </c>
       <c r="G4">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="H4">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I4">
         <v>31</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L4">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="M4">
-        <v>33</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>42600.830787037034</v>
+        <v>42604.890416666669</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5">
-        <v>6736</v>
+        <v>4034</v>
       </c>
       <c r="D5">
-        <v>8115</v>
+        <v>4529</v>
       </c>
       <c r="E5">
-        <v>956</v>
+        <v>571</v>
       </c>
       <c r="F5">
-        <v>111</v>
+        <v>49</v>
       </c>
       <c r="G5">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H5">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="I5">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="J5">
         <v>2</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L5">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="M5">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>42600.879189814812</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6">
-        <v>5830</v>
-      </c>
-      <c r="D6">
-        <v>6498</v>
-      </c>
-      <c r="E6">
-        <v>754</v>
-      </c>
-      <c r="F6">
-        <v>73</v>
-      </c>
-      <c r="G6">
-        <v>49</v>
-      </c>
-      <c r="H6">
-        <v>59</v>
-      </c>
-      <c r="I6">
-        <v>39</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>50</v>
-      </c>
-      <c r="M6">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>42602.582511574074</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>6203</v>
-      </c>
-      <c r="D7">
-        <v>9316</v>
-      </c>
-      <c r="E7">
-        <v>1145</v>
-      </c>
-      <c r="F7">
-        <v>133</v>
-      </c>
-      <c r="G7">
-        <v>61</v>
-      </c>
-      <c r="H7">
-        <v>67</v>
-      </c>
-      <c r="I7">
-        <v>31</v>
-      </c>
-      <c r="J7">
-        <v>3</v>
-      </c>
-      <c r="K7">
-        <v>3</v>
-      </c>
-      <c r="L7">
-        <v>49</v>
-      </c>
-      <c r="M7">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>42604.890416666669</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8">
-        <v>4034</v>
-      </c>
-      <c r="D8">
-        <v>4529</v>
-      </c>
-      <c r="E8">
-        <v>571</v>
-      </c>
-      <c r="F8">
-        <v>49</v>
-      </c>
-      <c r="G8">
-        <v>61</v>
-      </c>
-      <c r="H8">
-        <v>44</v>
-      </c>
-      <c r="I8">
-        <v>54</v>
-      </c>
-      <c r="J8">
-        <v>2</v>
-      </c>
-      <c r="K8">
-        <v>8</v>
-      </c>
-      <c r="L8">
-        <v>20</v>
-      </c>
-      <c r="M8">
         <v>80</v>
       </c>
     </row>

</xml_diff>